<commit_message>
Modificat ruta QR în /scan
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -677,9 +677,38 @@
         <v>Curs</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Alexia</v>
+      </c>
+      <c r="B11" t="str">
+        <v>ioana-alexia.badea27@s.fpse.unibuc.ro</v>
+      </c>
+      <c r="C11" t="str">
+        <v>25.04.2025</v>
+      </c>
+      <c r="D11" t="str">
+        <v>21:44:30</v>
+      </c>
+      <c r="E11" t="str">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <v>2</v>
+      </c>
+      <c r="G11" t="str">
+        <v>3</v>
+      </c>
+      <c r="H11" t="str">
+        <v>TMI II</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Seminar</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>